<commit_message>
Elimine un archivo, modifique 2archivos y agg un nuevo archivo
</commit_message>
<xml_diff>
--- a/Calculo_Cai.xlsx
+++ b/Calculo_Cai.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UTE LVT PC#7\Documents\Mi_destino_Caicedo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UTE LVT PC#7\Documents\Mi_Destino_Caicedo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD54879-9282-4427-AA16-CA1AA36486CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FB3FF9-4B88-473A-9EA8-BA833E29CF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BBD330D6-5910-4841-BF93-DD9278BD2E27}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>calculo de la nota</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>Leroy Caicedo</t>
   </si>
 </sst>
 </file>
@@ -389,20 +392,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC1EA4B-C93B-4FAE-89A6-68F95907EE31}">
-  <dimension ref="A2:C8"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -414,7 +417,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -426,7 +429,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -435,10 +438,15 @@
         <v>8.5500000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <f>ROUND(C7,0)</f>
         <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>